<commit_message>
Initial PeriodManager React version
</commit_message>
<xml_diff>
--- a/React/LearnThaiLanguage/Design.xlsx
+++ b/React/LearnThaiLanguage/Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3358,6 +3358,44 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>350950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>178233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Picture 106"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5778500" y="1333500"/>
+          <a:ext cx="350950" cy="368733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6818,6 +6856,159 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>398780</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50295</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="Rectangle 127"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="2286000"/>
+          <a:ext cx="2875280" cy="4634995"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="20000">
+              <a:srgbClr val="CCFFCC"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3366FF"/>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="60000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="100000" t="100000"/>
+          </a:path>
+          <a:tileRect r="-100000" b="-100000"/>
+        </a:gradFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381233</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>55274</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="Rectangle 128"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="749300"/>
+          <a:ext cx="2857733" cy="448974"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="7F7F7F"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7145,8 +7336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7166,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>